<commit_message>
implement registration for seller, admin, buyer, approval
</commit_message>
<xml_diff>
--- a/FinalProject/Schedule/Task Assignments.xlsx
+++ b/FinalProject/Schedule/Task Assignments.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GitHub\WAA\FinalProject\Schedule\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7BC7ABC3-07D1-498F-BA63-4F0349E3F6B3}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C64892C5-9DF2-4E2B-8421-53A28881795D}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="10545" activeTab="1" xr2:uid="{E955D212-A420-493E-B11A-13DB1F909248}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="10545" xr2:uid="{E955D212-A420-493E-B11A-13DB1F909248}"/>
   </bookViews>
   <sheets>
     <sheet name="Front End" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="27">
   <si>
     <t>Task</t>
   </si>
@@ -76,9 +76,6 @@
     <t>Product Controller</t>
   </si>
   <si>
-    <t>Implement apis for product: list product, product details</t>
-  </si>
-  <si>
     <t>Ly Sa</t>
   </si>
   <si>
@@ -95,6 +92,21 @@
   </si>
   <si>
     <t>Vivek</t>
+  </si>
+  <si>
+    <t>Admin controller</t>
+  </si>
+  <si>
+    <t>apis for approve seller</t>
+  </si>
+  <si>
+    <t>Implement apis for product: list product, product details,create new product</t>
+  </si>
+  <si>
+    <t>Create Product</t>
+  </si>
+  <si>
+    <t>Seller is allowed to post new product</t>
   </si>
 </sst>
 </file>
@@ -449,10 +461,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E72C815C-F306-4F1B-BE61-9B9FC8877A45}">
-  <dimension ref="A1:D9"/>
+  <dimension ref="A1:D10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -519,14 +531,22 @@
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>11</v>
+        <v>25</v>
       </c>
       <c r="B8" t="s">
-        <v>13</v>
+        <v>26</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
+        <v>11</v>
+      </c>
+      <c r="B9" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
         <v>12</v>
       </c>
     </row>
@@ -537,10 +557,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2270EE3E-E91D-4A72-8C3E-613A07A5574D}">
-  <dimension ref="A1:D4"/>
+  <dimension ref="A1:D5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -570,32 +590,40 @@
         <v>15</v>
       </c>
       <c r="B2" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C2" t="s">
         <v>16</v>
-      </c>
-      <c r="C2" t="s">
-        <v>17</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B3" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C3" t="s">
         <v>21</v>
-      </c>
-      <c r="C3" t="s">
-        <v>22</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
+        <v>18</v>
+      </c>
+      <c r="B4" t="s">
         <v>19</v>
       </c>
-      <c r="B4" t="s">
-        <v>20</v>
-      </c>
       <c r="C4" t="s">
-        <v>17</v>
+        <v>16</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>22</v>
+      </c>
+      <c r="B5" t="s">
+        <v>23</v>
       </c>
     </row>
   </sheetData>

</xml_diff>